<commit_message>
created exp. timeline, added Clam Bay temperature data from June 2018 to June 2019
</commit_message>
<xml_diff>
--- a/data/Oly 2018 Feeding Temperature Daily Log.xlsx
+++ b/data/Oly 2018 Feeding Temperature Daily Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura/Documents/roberts-lab/O.lurida_Temperature/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1C23F8-F629-FF46-84E6-2A54D9F70EB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27414632-40BC-D84A-ADBC-18D3FBAD41BA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13960" yWindow="460" windowWidth="14640" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,6 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -252,7 +253,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -301,8 +302,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1078,7 +1079,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1399,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O75"/>
+  <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1419,7 +1420,7 @@
     <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1461,7 +1462,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>43076</v>
       </c>
@@ -1502,8 +1503,16 @@
         <f>200-N2</f>
         <v>182</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2">
+        <f>SUM(O2,M2)</f>
+        <v>196</v>
+      </c>
+      <c r="Q2">
+        <f>P2/3</f>
+        <v>65.333333333333329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>43081</v>
       </c>
@@ -1544,8 +1553,16 @@
         <f>200-N3</f>
         <v>181</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3">
+        <f>SUM(O3,M3)</f>
+        <v>186</v>
+      </c>
+      <c r="Q3">
+        <f>P3/3</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>43082</v>
       </c>
@@ -1589,8 +1606,16 @@
         <f>200-N4</f>
         <v>169</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4">
+        <f>SUM(O4,M4)</f>
+        <v>192</v>
+      </c>
+      <c r="Q4">
+        <f>P4/3</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>43082</v>
       </c>
@@ -1631,8 +1656,16 @@
         <f>200-N5</f>
         <v>178</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5">
+        <f>SUM(O5,M5)</f>
+        <v>191</v>
+      </c>
+      <c r="Q5">
+        <f>P5/3</f>
+        <v>63.666666666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>43082</v>
       </c>
@@ -1652,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>43089</v>
       </c>
@@ -1672,7 +1705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>43095</v>
       </c>
@@ -1692,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>43095</v>
       </c>
@@ -1712,7 +1745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>43095</v>
       </c>
@@ -1732,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>43096</v>
       </c>
@@ -1749,7 +1782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>43102</v>
       </c>
@@ -1769,7 +1802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>43102</v>
       </c>
@@ -1789,7 +1822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>43102</v>
       </c>
@@ -1809,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>43103</v>
       </c>
@@ -1826,7 +1859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>43116</v>
       </c>

</xml_diff>